<commit_message>
Updated readme, correct host LED connections in schematic, added Xbee programmer to BOM.
</commit_message>
<xml_diff>
--- a/sch/BOM.xlsx
+++ b/sch/BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>82T9863</t>
   </si>
@@ -236,6 +236,13 @@
   </si>
   <si>
     <t>RES 100 OHM 1/4W 5% CARBON FILM (current control for button LED)</t>
+  </si>
+  <si>
+    <t>WRL-11812</t>
+  </si>
+  <si>
+    <t>SparkFun XBee Explorer USB (used to program the Xbee module)
+http://www.sparkfun.com/products/11812</t>
   </si>
 </sst>
 </file>
@@ -1130,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G41"/>
+  <dimension ref="A2:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,7 +1227,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G19" si="0">F5*E5</f>
+        <f t="shared" ref="G5:G20" si="0">F5*E5</f>
         <v>0.17699999999999999</v>
       </c>
     </row>
@@ -1329,12 +1336,12 @@
         <v>19.649999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>27</v>
@@ -1343,61 +1350,61 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1.95</v>
+        <v>24.95</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>1.95</v>
+        <v>24.95</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E12">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>8.8200000000000001E-2</v>
+        <v>1.95</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
-        <v>2.8224</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F13">
-        <v>0.7</v>
+        <v>8.8200000000000001E-2</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>2.8224</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>21</v>
@@ -1406,19 +1413,19 @@
         <v>4</v>
       </c>
       <c r="F14">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>21</v>
@@ -1427,19 +1434,19 @@
         <v>4</v>
       </c>
       <c r="F15">
-        <v>0.62</v>
+        <v>0.9</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="0"/>
-        <v>2.48</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>21</v>
@@ -1448,150 +1455,150 @@
         <v>4</v>
       </c>
       <c r="F16">
-        <v>0.77</v>
+        <v>0.62</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="0"/>
-        <v>3.08</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="9">
-        <v>1281</v>
+      <c r="B17" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F17">
-        <v>24.95</v>
+        <v>0.77</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="0"/>
-        <v>24.95</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
-        <v>31004</v>
+      <c r="B18" s="9">
+        <v>1281</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>13.99</v>
+        <v>24.95</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="0"/>
-        <v>41.97</v>
+        <v>24.95</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
-        <v>80005</v>
+        <v>31004</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>2.2799999999999998</v>
+        <v>13.99</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
+        <v>41.97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
+        <v>80005</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
         <v>9.1199999999999992</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="1"/>
-    </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F21" s="10" t="s">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="4">
-        <f>SUM(G4:G19)</f>
-        <v>384.80240000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="G22" s="4">
+        <f>SUM(G4:G20)</f>
+        <v>409.75239999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
-      </c>
-      <c r="F25">
-        <v>18.72</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" ref="G25:G38" si="1">F25*E25</f>
-        <v>56.16</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>8</v>
@@ -1603,229 +1610,229 @@
         <v>3</v>
       </c>
       <c r="F26">
+        <v>18.72</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" ref="G26:G39" si="1">F26*E26</f>
+        <v>56.16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
         <v>15.92</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G27" s="1">
         <f t="shared" si="1"/>
         <v>47.76</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>1</v>
       </c>
-      <c r="F27">
+      <c r="F28">
         <v>18.829999999999998</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G28" s="1">
         <f t="shared" si="1"/>
         <v>18.829999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>3</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>12.8</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G29" s="1">
         <f t="shared" si="1"/>
         <v>38.400000000000006</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <v>3</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>4.8099999999999996</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G30" s="1">
         <f t="shared" si="1"/>
         <v>14.43</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>3</v>
       </c>
-      <c r="F30">
+      <c r="F31">
         <v>3.15</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G31" s="1">
         <f t="shared" si="1"/>
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>3</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F32" s="1">
         <v>8.1</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G32" s="1">
         <f t="shared" si="1"/>
         <v>24.299999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>2</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>9.16</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G33" s="1">
         <f t="shared" si="1"/>
         <v>18.32</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="8" t="s">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>2</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <v>15.32</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G34" s="1">
         <f t="shared" si="1"/>
         <v>30.64</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="8" t="s">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <v>1</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>24.99</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G35" s="1">
         <f t="shared" si="1"/>
         <v>24.99</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <v>1</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <v>30</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G36" s="1">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36">
-        <v>3</v>
-      </c>
-      <c r="F36">
-        <v>19.95</v>
-      </c>
-      <c r="G36" s="1">
-        <f t="shared" si="1"/>
-        <v>59.849999999999994</v>
-      </c>
-    </row>
     <row r="37" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>61</v>
@@ -1843,47 +1850,68 @@
     </row>
     <row r="38" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E38">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F38">
-        <v>1.95</v>
+        <v>19.95</v>
       </c>
       <c r="G38" s="1">
         <f t="shared" si="1"/>
+        <v>59.849999999999994</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39">
+        <v>6</v>
+      </c>
+      <c r="F39">
+        <v>1.95</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="1"/>
         <v>11.7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F40" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G40" s="4">
-        <f>SUM(G25:G38)</f>
-        <v>444.68</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F41" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" s="4">
+        <f>SUM(G26:G39)</f>
+        <v>444.68</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G41" s="4">
-        <f>SUM(G21,G40)</f>
-        <v>829.4824000000001</v>
+      <c r="G42" s="4">
+        <f>SUM(G22,G41)</f>
+        <v>854.43239999999992</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>